<commit_message>
add new Rachel neut data for 557
</commit_message>
<xml_diff>
--- a/data/neut_assays/plate_reader_data/557v1_NeutralizationAssay.xlsx
+++ b/data/neut_assays/plate_reader_data/557v1_NeutralizationAssay.xlsx
@@ -1,29 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhyemlee/Google Drive/Bloom_Lab/Perth2009_MAP/NeutralizationAssays/mutvalidation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30820" yWindow="460" windowWidth="29020" windowHeight="17600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WT" sheetId="2" r:id="rId1"/>
     <sheet name="F159G" sheetId="1" r:id="rId2"/>
     <sheet name="R220D" sheetId="3" r:id="rId3"/>
     <sheet name="K189D" sheetId="4" r:id="rId4"/>
+    <sheet name="WT-2" sheetId="5" r:id="rId5"/>
+    <sheet name="F159G-2" sheetId="6" r:id="rId6"/>
+    <sheet name="R220D-2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -385,8 +383,275 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="74">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -572,6 +837,42 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>11:39:00 AM</t>
+  </si>
+  <si>
+    <t>FHCRC\reguia</t>
+  </si>
+  <si>
+    <t>6/5/2019 11:40:01 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 24.1 °C</t>
+  </si>
+  <si>
+    <t>6/5/2019 11:40:57 AM</t>
+  </si>
+  <si>
+    <t>11:36:39 AM</t>
+  </si>
+  <si>
+    <t>6/5/2019 11:37:40 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 23.8 °C</t>
+  </si>
+  <si>
+    <t>6/5/2019 11:38:36 AM</t>
+  </si>
+  <si>
+    <t>11:34:07 AM</t>
+  </si>
+  <si>
+    <t>6/5/2019 11:35:13 AM</t>
+  </si>
+  <si>
+    <t>6/5/2019 11:36:09 AM</t>
   </si>
 </sst>
 </file>
@@ -751,7 +1052,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -786,7 +1087,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -997,13 +1298,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1019,7 +1320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1027,7 +1328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1035,7 +1336,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1043,7 +1344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1051,7 +1352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1059,7 +1360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1067,17 +1368,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1085,12 +1386,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1101,7 +1402,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1112,7 +1413,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1123,7 +1424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1134,7 +1435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1145,7 +1446,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1156,7 +1457,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1167,7 +1468,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1178,7 +1479,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1189,7 +1490,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1200,7 +1501,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1208,12 +1509,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1254,12 +1555,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1300,7 +1601,7 @@
         <v>10546</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1341,7 +1642,7 @@
         <v>28994</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1382,7 +1683,7 @@
         <v>14598</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -1423,7 +1724,7 @@
         <v>14691</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -1464,7 +1765,7 @@
         <v>14539</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -1505,12 +1806,12 @@
         <v>29391</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1521,6 +1822,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1532,9 +1838,9 @@
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1542,7 +1848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1550,7 +1856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1558,7 +1864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1566,7 +1872,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1880,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1582,7 +1888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1590,7 +1896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1598,17 +1904,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1616,12 +1922,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1632,7 +1938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1643,7 +1949,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1654,7 +1960,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1665,7 +1971,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1676,7 +1982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1687,7 +1993,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1698,7 +2004,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1709,7 +2015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1720,7 +2026,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1731,7 +2037,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1739,12 +2045,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1785,12 +2091,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1831,7 +2137,7 @@
         <v>6906</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1872,7 +2178,7 @@
         <v>28127</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1913,7 +2219,7 @@
         <v>34485</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -1954,7 +2260,7 @@
         <v>33324</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -1995,7 +2301,7 @@
         <v>33465</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2036,12 +2342,12 @@
         <v>27476</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2052,6 +2358,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2063,9 +2374,9 @@
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2073,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2081,7 +2392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2089,7 +2400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2097,7 +2408,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2105,7 +2416,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2113,7 +2424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2121,7 +2432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2129,17 +2440,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2147,12 +2458,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2163,7 +2474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2174,7 +2485,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2185,7 +2496,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2196,7 +2507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2207,7 +2518,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2218,7 +2529,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2229,7 +2540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2240,7 +2551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2251,7 +2562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2262,7 +2573,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2270,12 +2581,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2316,12 +2627,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -2362,7 +2673,7 @@
         <v>8822</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -2403,7 +2714,7 @@
         <v>27290</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -2444,7 +2755,7 @@
         <v>11210</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -2485,7 +2796,7 @@
         <v>11648</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -2526,7 +2837,7 @@
         <v>11397</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2567,12 +2878,12 @@
         <v>27291</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2583,6 +2894,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2594,9 +2910,9 @@
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2604,7 +2920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2612,7 +2928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2620,7 +2936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2628,7 +2944,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2636,7 +2952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2644,7 +2960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2652,7 +2968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2660,17 +2976,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2678,12 +2994,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2694,7 +3010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2705,7 +3021,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2716,7 +3032,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2727,7 +3043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2738,7 +3054,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2749,7 +3065,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2760,7 +3076,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2771,7 +3087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2782,7 +3098,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2793,7 +3109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2801,12 +3117,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2847,12 +3163,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -2893,7 +3209,7 @@
         <v>10279</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -2934,7 +3250,7 @@
         <v>28762</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -2975,7 +3291,7 @@
         <v>13004</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -3016,7 +3332,7 @@
         <v>13347</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -3057,7 +3373,7 @@
         <v>13306</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -3098,12 +3414,12 @@
         <v>20660</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -3114,5 +3430,1834 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>92</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>4059</v>
+      </c>
+      <c r="C32">
+        <v>4079</v>
+      </c>
+      <c r="D32">
+        <v>4177</v>
+      </c>
+      <c r="E32">
+        <v>4309</v>
+      </c>
+      <c r="F32">
+        <v>4393</v>
+      </c>
+      <c r="G32">
+        <v>4424</v>
+      </c>
+      <c r="H32">
+        <v>4388</v>
+      </c>
+      <c r="I32">
+        <v>4398</v>
+      </c>
+      <c r="J32">
+        <v>4265</v>
+      </c>
+      <c r="K32">
+        <v>4190</v>
+      </c>
+      <c r="L32">
+        <v>4106</v>
+      </c>
+      <c r="M32">
+        <v>3945</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>7037</v>
+      </c>
+      <c r="C33">
+        <v>7120</v>
+      </c>
+      <c r="D33">
+        <v>7132</v>
+      </c>
+      <c r="E33">
+        <v>7275</v>
+      </c>
+      <c r="F33">
+        <v>7266</v>
+      </c>
+      <c r="G33">
+        <v>7314</v>
+      </c>
+      <c r="H33">
+        <v>7285</v>
+      </c>
+      <c r="I33">
+        <v>7258</v>
+      </c>
+      <c r="J33">
+        <v>7207</v>
+      </c>
+      <c r="K33">
+        <v>7186</v>
+      </c>
+      <c r="L33">
+        <v>7061</v>
+      </c>
+      <c r="M33">
+        <v>7145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>24327</v>
+      </c>
+      <c r="C34">
+        <v>30360</v>
+      </c>
+      <c r="D34">
+        <v>33736</v>
+      </c>
+      <c r="E34">
+        <v>33592</v>
+      </c>
+      <c r="F34">
+        <v>36375</v>
+      </c>
+      <c r="G34">
+        <v>36025</v>
+      </c>
+      <c r="H34">
+        <v>36168</v>
+      </c>
+      <c r="I34">
+        <v>37429</v>
+      </c>
+      <c r="J34">
+        <v>35727</v>
+      </c>
+      <c r="K34">
+        <v>35929</v>
+      </c>
+      <c r="L34">
+        <v>33319</v>
+      </c>
+      <c r="M34">
+        <v>25453</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>24772</v>
+      </c>
+      <c r="C35">
+        <v>31253</v>
+      </c>
+      <c r="D35">
+        <v>35349</v>
+      </c>
+      <c r="E35">
+        <v>33466</v>
+      </c>
+      <c r="F35">
+        <v>36641</v>
+      </c>
+      <c r="G35">
+        <v>36051</v>
+      </c>
+      <c r="H35">
+        <v>33101</v>
+      </c>
+      <c r="I35">
+        <v>26340</v>
+      </c>
+      <c r="J35">
+        <v>13725</v>
+      </c>
+      <c r="K35">
+        <v>7619</v>
+      </c>
+      <c r="L35">
+        <v>8161</v>
+      </c>
+      <c r="M35">
+        <v>10120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>23300</v>
+      </c>
+      <c r="C36">
+        <v>31905</v>
+      </c>
+      <c r="D36">
+        <v>33617</v>
+      </c>
+      <c r="E36">
+        <v>34158</v>
+      </c>
+      <c r="F36">
+        <v>34109</v>
+      </c>
+      <c r="G36">
+        <v>33702</v>
+      </c>
+      <c r="H36">
+        <v>32530</v>
+      </c>
+      <c r="I36">
+        <v>25830</v>
+      </c>
+      <c r="J36">
+        <v>12239</v>
+      </c>
+      <c r="K36">
+        <v>7651</v>
+      </c>
+      <c r="L36">
+        <v>8104</v>
+      </c>
+      <c r="M36">
+        <v>9994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>21896</v>
+      </c>
+      <c r="C37">
+        <v>31571</v>
+      </c>
+      <c r="D37">
+        <v>29983</v>
+      </c>
+      <c r="E37">
+        <v>33282</v>
+      </c>
+      <c r="F37">
+        <v>34311</v>
+      </c>
+      <c r="G37">
+        <v>33272</v>
+      </c>
+      <c r="H37">
+        <v>31711</v>
+      </c>
+      <c r="I37">
+        <v>23977</v>
+      </c>
+      <c r="J37">
+        <v>12539</v>
+      </c>
+      <c r="K37">
+        <v>7733</v>
+      </c>
+      <c r="L37">
+        <v>8039</v>
+      </c>
+      <c r="M37">
+        <v>9770</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>20352</v>
+      </c>
+      <c r="C38">
+        <v>29095</v>
+      </c>
+      <c r="D38">
+        <v>28347</v>
+      </c>
+      <c r="E38">
+        <v>27996</v>
+      </c>
+      <c r="F38">
+        <v>30990</v>
+      </c>
+      <c r="G38">
+        <v>30729</v>
+      </c>
+      <c r="H38">
+        <v>31143</v>
+      </c>
+      <c r="I38">
+        <v>31382</v>
+      </c>
+      <c r="J38">
+        <v>29511</v>
+      </c>
+      <c r="K38">
+        <v>29754</v>
+      </c>
+      <c r="L38">
+        <v>27291</v>
+      </c>
+      <c r="M38">
+        <v>24348</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39">
+        <v>3610</v>
+      </c>
+      <c r="C39">
+        <v>3662</v>
+      </c>
+      <c r="D39">
+        <v>3823</v>
+      </c>
+      <c r="E39">
+        <v>3894</v>
+      </c>
+      <c r="F39">
+        <v>3976</v>
+      </c>
+      <c r="G39">
+        <v>4025</v>
+      </c>
+      <c r="H39">
+        <v>4042</v>
+      </c>
+      <c r="I39">
+        <v>4014</v>
+      </c>
+      <c r="J39">
+        <v>3937</v>
+      </c>
+      <c r="K39">
+        <v>3819</v>
+      </c>
+      <c r="L39">
+        <v>3734</v>
+      </c>
+      <c r="M39">
+        <v>3631</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>89</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>3088</v>
+      </c>
+      <c r="C32">
+        <v>3117</v>
+      </c>
+      <c r="D32">
+        <v>3193</v>
+      </c>
+      <c r="E32">
+        <v>3261</v>
+      </c>
+      <c r="F32">
+        <v>3332</v>
+      </c>
+      <c r="G32">
+        <v>3353</v>
+      </c>
+      <c r="H32">
+        <v>3360</v>
+      </c>
+      <c r="I32">
+        <v>3355</v>
+      </c>
+      <c r="J32">
+        <v>3233</v>
+      </c>
+      <c r="K32">
+        <v>3197</v>
+      </c>
+      <c r="L32">
+        <v>3063</v>
+      </c>
+      <c r="M32">
+        <v>2934</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>4126</v>
+      </c>
+      <c r="C33">
+        <v>4132</v>
+      </c>
+      <c r="D33">
+        <v>4211</v>
+      </c>
+      <c r="E33">
+        <v>4316</v>
+      </c>
+      <c r="F33">
+        <v>4325</v>
+      </c>
+      <c r="G33">
+        <v>4361</v>
+      </c>
+      <c r="H33">
+        <v>4330</v>
+      </c>
+      <c r="I33">
+        <v>4349</v>
+      </c>
+      <c r="J33">
+        <v>4278</v>
+      </c>
+      <c r="K33">
+        <v>4155</v>
+      </c>
+      <c r="L33">
+        <v>4089</v>
+      </c>
+      <c r="M33">
+        <v>4069</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>19102</v>
+      </c>
+      <c r="C34">
+        <v>25068</v>
+      </c>
+      <c r="D34">
+        <v>28619</v>
+      </c>
+      <c r="E34">
+        <v>28954</v>
+      </c>
+      <c r="F34">
+        <v>31803</v>
+      </c>
+      <c r="G34">
+        <v>34541</v>
+      </c>
+      <c r="H34">
+        <v>33332</v>
+      </c>
+      <c r="I34">
+        <v>32954</v>
+      </c>
+      <c r="J34">
+        <v>33678</v>
+      </c>
+      <c r="K34">
+        <v>29908</v>
+      </c>
+      <c r="L34">
+        <v>29399</v>
+      </c>
+      <c r="M34">
+        <v>25785</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>20648</v>
+      </c>
+      <c r="C35">
+        <v>25504</v>
+      </c>
+      <c r="D35">
+        <v>28116</v>
+      </c>
+      <c r="E35">
+        <v>29163</v>
+      </c>
+      <c r="F35">
+        <v>31626</v>
+      </c>
+      <c r="G35">
+        <v>33953</v>
+      </c>
+      <c r="H35">
+        <v>34827</v>
+      </c>
+      <c r="I35">
+        <v>33857</v>
+      </c>
+      <c r="J35">
+        <v>32548</v>
+      </c>
+      <c r="K35">
+        <v>32969</v>
+      </c>
+      <c r="L35">
+        <v>37015</v>
+      </c>
+      <c r="M35">
+        <v>36518</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>23771</v>
+      </c>
+      <c r="C36">
+        <v>28394</v>
+      </c>
+      <c r="D36">
+        <v>27149</v>
+      </c>
+      <c r="E36">
+        <v>27099</v>
+      </c>
+      <c r="F36">
+        <v>29065</v>
+      </c>
+      <c r="G36">
+        <v>32362</v>
+      </c>
+      <c r="H36">
+        <v>32545</v>
+      </c>
+      <c r="I36">
+        <v>32136</v>
+      </c>
+      <c r="J36">
+        <v>33307</v>
+      </c>
+      <c r="K36">
+        <v>31999</v>
+      </c>
+      <c r="L36">
+        <v>34780</v>
+      </c>
+      <c r="M36">
+        <v>37351</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>22505</v>
+      </c>
+      <c r="C37">
+        <v>26582</v>
+      </c>
+      <c r="D37">
+        <v>27630</v>
+      </c>
+      <c r="E37">
+        <v>25881</v>
+      </c>
+      <c r="F37">
+        <v>25218</v>
+      </c>
+      <c r="G37">
+        <v>27824</v>
+      </c>
+      <c r="H37">
+        <v>31579</v>
+      </c>
+      <c r="I37">
+        <v>29820</v>
+      </c>
+      <c r="J37">
+        <v>30821</v>
+      </c>
+      <c r="K37">
+        <v>30582</v>
+      </c>
+      <c r="L37">
+        <v>31005</v>
+      </c>
+      <c r="M37">
+        <v>35712</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>18320</v>
+      </c>
+      <c r="C38">
+        <v>26402</v>
+      </c>
+      <c r="D38">
+        <v>26578</v>
+      </c>
+      <c r="E38">
+        <v>25173</v>
+      </c>
+      <c r="F38">
+        <v>23527</v>
+      </c>
+      <c r="G38">
+        <v>25662</v>
+      </c>
+      <c r="H38">
+        <v>26008</v>
+      </c>
+      <c r="I38">
+        <v>27307</v>
+      </c>
+      <c r="J38">
+        <v>26887</v>
+      </c>
+      <c r="K38">
+        <v>26426</v>
+      </c>
+      <c r="L38">
+        <v>26230</v>
+      </c>
+      <c r="M38">
+        <v>22021</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39">
+        <v>2779</v>
+      </c>
+      <c r="C39">
+        <v>2762</v>
+      </c>
+      <c r="D39">
+        <v>2907</v>
+      </c>
+      <c r="E39">
+        <v>2946</v>
+      </c>
+      <c r="F39">
+        <v>3009</v>
+      </c>
+      <c r="G39">
+        <v>3036</v>
+      </c>
+      <c r="H39">
+        <v>3039</v>
+      </c>
+      <c r="I39">
+        <v>3021</v>
+      </c>
+      <c r="J39">
+        <v>2954</v>
+      </c>
+      <c r="K39">
+        <v>2882</v>
+      </c>
+      <c r="L39">
+        <v>2807</v>
+      </c>
+      <c r="M39">
+        <v>2736</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>4041</v>
+      </c>
+      <c r="C32">
+        <v>4264</v>
+      </c>
+      <c r="D32">
+        <v>4470</v>
+      </c>
+      <c r="E32">
+        <v>4564</v>
+      </c>
+      <c r="F32">
+        <v>4635</v>
+      </c>
+      <c r="G32">
+        <v>4594</v>
+      </c>
+      <c r="H32">
+        <v>4670</v>
+      </c>
+      <c r="I32">
+        <v>4613</v>
+      </c>
+      <c r="J32">
+        <v>4539</v>
+      </c>
+      <c r="K32">
+        <v>4487</v>
+      </c>
+      <c r="L32">
+        <v>4281</v>
+      </c>
+      <c r="M32">
+        <v>4080</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>5921</v>
+      </c>
+      <c r="C33">
+        <v>5954</v>
+      </c>
+      <c r="D33">
+        <v>6172</v>
+      </c>
+      <c r="E33">
+        <v>6267</v>
+      </c>
+      <c r="F33">
+        <v>6342</v>
+      </c>
+      <c r="G33">
+        <v>6387</v>
+      </c>
+      <c r="H33">
+        <v>6395</v>
+      </c>
+      <c r="I33">
+        <v>6368</v>
+      </c>
+      <c r="J33">
+        <v>6257</v>
+      </c>
+      <c r="K33">
+        <v>6226</v>
+      </c>
+      <c r="L33">
+        <v>6102</v>
+      </c>
+      <c r="M33">
+        <v>5957</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>23150</v>
+      </c>
+      <c r="C34">
+        <v>27237</v>
+      </c>
+      <c r="D34">
+        <v>27597</v>
+      </c>
+      <c r="E34">
+        <v>28660</v>
+      </c>
+      <c r="F34">
+        <v>29998</v>
+      </c>
+      <c r="G34">
+        <v>30487</v>
+      </c>
+      <c r="H34">
+        <v>30339</v>
+      </c>
+      <c r="I34">
+        <v>30398</v>
+      </c>
+      <c r="J34">
+        <v>28802</v>
+      </c>
+      <c r="K34">
+        <v>28633</v>
+      </c>
+      <c r="L34">
+        <v>27898</v>
+      </c>
+      <c r="M34">
+        <v>23202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>23221</v>
+      </c>
+      <c r="C35">
+        <v>29126</v>
+      </c>
+      <c r="D35">
+        <v>28918</v>
+      </c>
+      <c r="E35">
+        <v>30146</v>
+      </c>
+      <c r="F35">
+        <v>30781</v>
+      </c>
+      <c r="G35">
+        <v>34240</v>
+      </c>
+      <c r="H35">
+        <v>36386</v>
+      </c>
+      <c r="I35">
+        <v>37645</v>
+      </c>
+      <c r="J35">
+        <v>35824</v>
+      </c>
+      <c r="K35">
+        <v>35963</v>
+      </c>
+      <c r="L35">
+        <v>19242</v>
+      </c>
+      <c r="M35">
+        <v>9575</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>21300</v>
+      </c>
+      <c r="C36">
+        <v>25407</v>
+      </c>
+      <c r="D36">
+        <v>27482</v>
+      </c>
+      <c r="E36">
+        <v>28868</v>
+      </c>
+      <c r="F36">
+        <v>30886</v>
+      </c>
+      <c r="G36">
+        <v>33118</v>
+      </c>
+      <c r="H36">
+        <v>35451</v>
+      </c>
+      <c r="I36">
+        <v>37632</v>
+      </c>
+      <c r="J36">
+        <v>35807</v>
+      </c>
+      <c r="K36">
+        <v>33741</v>
+      </c>
+      <c r="L36">
+        <v>19913</v>
+      </c>
+      <c r="M36">
+        <v>9324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>20253</v>
+      </c>
+      <c r="C37">
+        <v>23924</v>
+      </c>
+      <c r="D37">
+        <v>25501</v>
+      </c>
+      <c r="E37">
+        <v>26583</v>
+      </c>
+      <c r="F37">
+        <v>30147</v>
+      </c>
+      <c r="G37">
+        <v>31968</v>
+      </c>
+      <c r="H37">
+        <v>33116</v>
+      </c>
+      <c r="I37">
+        <v>34523</v>
+      </c>
+      <c r="J37">
+        <v>33592</v>
+      </c>
+      <c r="K37">
+        <v>34458</v>
+      </c>
+      <c r="L37">
+        <v>18374</v>
+      </c>
+      <c r="M37">
+        <v>9410</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>18511</v>
+      </c>
+      <c r="C38">
+        <v>20884</v>
+      </c>
+      <c r="D38">
+        <v>22623</v>
+      </c>
+      <c r="E38">
+        <v>22610</v>
+      </c>
+      <c r="F38">
+        <v>23786</v>
+      </c>
+      <c r="G38">
+        <v>25226</v>
+      </c>
+      <c r="H38">
+        <v>25876</v>
+      </c>
+      <c r="I38">
+        <v>25360</v>
+      </c>
+      <c r="J38">
+        <v>24506</v>
+      </c>
+      <c r="K38">
+        <v>26677</v>
+      </c>
+      <c r="L38">
+        <v>24405</v>
+      </c>
+      <c r="M38">
+        <v>21518</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39">
+        <v>3788</v>
+      </c>
+      <c r="C39">
+        <v>3806</v>
+      </c>
+      <c r="D39">
+        <v>3941</v>
+      </c>
+      <c r="E39">
+        <v>4052</v>
+      </c>
+      <c r="F39">
+        <v>4310</v>
+      </c>
+      <c r="G39">
+        <v>4101</v>
+      </c>
+      <c r="H39">
+        <v>4271</v>
+      </c>
+      <c r="I39">
+        <v>4214</v>
+      </c>
+      <c r="J39">
+        <v>4075</v>
+      </c>
+      <c r="K39">
+        <v>3969</v>
+      </c>
+      <c r="L39">
+        <v>3887</v>
+      </c>
+      <c r="M39">
+        <v>3746</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>